<commit_message>
All results collected for data with and without brigthness
</commit_message>
<xml_diff>
--- a/P3/Results/Data/Clay/AllOTResults.xlsx
+++ b/P3/Results/Data/Clay/AllOTResults.xlsx
@@ -1,32 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Clay0.5g" sheetId="1" r:id="rId1"/>
+    <sheet name="Clay0.5g" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Clay1g" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Clay10g" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -45,13 +48,80 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -339,13 +409,965 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="65" customWidth="1" min="1" max="1"/>
+    <col width="44" customWidth="1" min="2" max="2"/>
+    <col width="43" customWidth="1" min="3" max="3"/>
+    <col width="27" customWidth="1" min="4" max="4"/>
+    <col width="26" customWidth="1" min="5" max="5"/>
+    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="11" customWidth="1" min="7" max="7"/>
+    <col width="14" customWidth="1" min="8" max="8"/>
+    <col width="13" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Filename</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>PSNR Ground checker diff Reference checker</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>PSNR Ground checker diff Enhanced checker</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Reference</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Enhanced</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Dehazed</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>AG Ground</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>AG Reference</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>AG Enhanced</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>AG Dehazed</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Beside_Camera_light10_exp78730.0_20242111_114101.png</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>10.71</v>
+      </c>
+      <c r="C2" t="n">
+        <v>16.57</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-33.7</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-10.93</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-6.36</v>
+      </c>
+      <c r="G2" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H2" t="n">
+        <v>3.48</v>
+      </c>
+      <c r="I2" t="n">
+        <v>18.98</v>
+      </c>
+      <c r="J2" t="n">
+        <v>17.33</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Beside_Camera_light5_exp121296.0_20242111_114135.png</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>11.16</v>
+      </c>
+      <c r="C3" t="n">
+        <v>16.33</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-36.59</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-9.99</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-5.94</v>
+      </c>
+      <c r="G3" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H3" t="n">
+        <v>3.73</v>
+      </c>
+      <c r="I3" t="n">
+        <v>18.02</v>
+      </c>
+      <c r="J3" t="n">
+        <v>16.7</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Green_Beside_Camera_light10_exp158798.0_20242111_114622.png</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>11.18</v>
+      </c>
+      <c r="C4" t="n">
+        <v>16.29</v>
+      </c>
+      <c r="D4" t="n">
+        <v>-40.5</v>
+      </c>
+      <c r="E4" t="n">
+        <v>-8.99</v>
+      </c>
+      <c r="F4" t="n">
+        <v>-6.64</v>
+      </c>
+      <c r="G4" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H4" t="n">
+        <v>4.09</v>
+      </c>
+      <c r="I4" t="n">
+        <v>19.43</v>
+      </c>
+      <c r="J4" t="n">
+        <v>16.05</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Green_Beside_Camera_light5_exp195346.0_20242111_114652.png</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>11.59</v>
+      </c>
+      <c r="C5" t="n">
+        <v>16.29</v>
+      </c>
+      <c r="D5" t="n">
+        <v>-38.31</v>
+      </c>
+      <c r="E5" t="n">
+        <v>-8.83</v>
+      </c>
+      <c r="F5" t="n">
+        <v>-4.94</v>
+      </c>
+      <c r="G5" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H5" t="n">
+        <v>4.21</v>
+      </c>
+      <c r="I5" t="n">
+        <v>19.35</v>
+      </c>
+      <c r="J5" t="n">
+        <v>15.57</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Green_InFront_Camera_light10_exp95037.0_20242111_114831.png</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>9.140000000000001</v>
+      </c>
+      <c r="C6" t="n">
+        <v>9.43</v>
+      </c>
+      <c r="D6" t="n">
+        <v>-39.23</v>
+      </c>
+      <c r="E6" t="n">
+        <v>-38.4</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-0.9</v>
+      </c>
+      <c r="G6" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H6" t="n">
+        <v>4.07</v>
+      </c>
+      <c r="I6" t="n">
+        <v>38.02</v>
+      </c>
+      <c r="J6" t="n">
+        <v>12.29</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Green_InFront_Camera_light5_exp148588.0_20242111_114858.png</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>10.72</v>
+      </c>
+      <c r="C7" t="n">
+        <v>15.23</v>
+      </c>
+      <c r="D7" t="n">
+        <v>-41.85</v>
+      </c>
+      <c r="E7" t="n">
+        <v>-22.15</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-4.17</v>
+      </c>
+      <c r="G7" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H7" t="n">
+        <v>4.28</v>
+      </c>
+      <c r="I7" t="n">
+        <v>24.8</v>
+      </c>
+      <c r="J7" t="n">
+        <v>13.82</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Green_Right_Side_light10_exp130235.0_20242111_114754.png</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>10.8</v>
+      </c>
+      <c r="C8" t="n">
+        <v>15.81</v>
+      </c>
+      <c r="D8" t="n">
+        <v>-39.94</v>
+      </c>
+      <c r="E8" t="n">
+        <v>-6.88</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-5.42</v>
+      </c>
+      <c r="G8" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H8" t="n">
+        <v>4.18</v>
+      </c>
+      <c r="I8" t="n">
+        <v>20.03</v>
+      </c>
+      <c r="J8" t="n">
+        <v>15.63</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Green_Right_Side_light5_exp175761.0_20242111_114725.png</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>11.43</v>
+      </c>
+      <c r="C9" t="n">
+        <v>16.41</v>
+      </c>
+      <c r="D9" t="n">
+        <v>-39.69</v>
+      </c>
+      <c r="E9" t="n">
+        <v>-6.96</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-6.01</v>
+      </c>
+      <c r="G9" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H9" t="n">
+        <v>4.26</v>
+      </c>
+      <c r="I9" t="n">
+        <v>18.4</v>
+      </c>
+      <c r="J9" t="n">
+        <v>15.91</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>InFront_Camera_light10_exp46155.0_20242111_114316.png</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>9.26</v>
+      </c>
+      <c r="C10" t="n">
+        <v>8.94</v>
+      </c>
+      <c r="D10" t="n">
+        <v>-35.4</v>
+      </c>
+      <c r="E10" t="n">
+        <v>-6.48</v>
+      </c>
+      <c r="F10" t="n">
+        <v>-2.62</v>
+      </c>
+      <c r="G10" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H10" t="n">
+        <v>3.76</v>
+      </c>
+      <c r="I10" t="n">
+        <v>57.96</v>
+      </c>
+      <c r="J10" t="n">
+        <v>13.33</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>InFront_Camera_light5_exp78134.0_20242111_114342.png</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>10.22</v>
+      </c>
+      <c r="C11" t="n">
+        <v>12.54</v>
+      </c>
+      <c r="D11" t="n">
+        <v>-35.48</v>
+      </c>
+      <c r="E11" t="n">
+        <v>-32.31</v>
+      </c>
+      <c r="F11" t="n">
+        <v>-3.44</v>
+      </c>
+      <c r="G11" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H11" t="n">
+        <v>3.84</v>
+      </c>
+      <c r="I11" t="n">
+        <v>35.68</v>
+      </c>
+      <c r="J11" t="n">
+        <v>13.85</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Right_Side_light10_exp54398.0_20242111_114233.png</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>11.01</v>
+      </c>
+      <c r="C12" t="n">
+        <v>15.2</v>
+      </c>
+      <c r="D12" t="n">
+        <v>-30.45</v>
+      </c>
+      <c r="E12" t="n">
+        <v>-7.98</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.86</v>
+      </c>
+      <c r="G12" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H12" t="n">
+        <v>3.93</v>
+      </c>
+      <c r="I12" t="n">
+        <v>17.77</v>
+      </c>
+      <c r="J12" t="n">
+        <v>13.96</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Right_Side_light5_exp90409.0_20242111_114207.png</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>11.23</v>
+      </c>
+      <c r="C13" t="n">
+        <v>15.72</v>
+      </c>
+      <c r="D13" t="n">
+        <v>-32.04</v>
+      </c>
+      <c r="E13" t="n">
+        <v>-7.99</v>
+      </c>
+      <c r="F13" t="n">
+        <v>-0.93</v>
+      </c>
+      <c r="G13" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H13" t="n">
+        <v>3.89</v>
+      </c>
+      <c r="I13" t="n">
+        <v>17.73</v>
+      </c>
+      <c r="J13" t="n">
+        <v>14.7</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Underwater_Beside_Camera_lightx_exp197034.0_20242111_114428.png</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>11.26</v>
+      </c>
+      <c r="C14" t="n">
+        <v>16.14</v>
+      </c>
+      <c r="D14" t="n">
+        <v>-37.12</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="F14" t="n">
+        <v>-0.17</v>
+      </c>
+      <c r="G14" t="n">
+        <v>8.619999999999999</v>
+      </c>
+      <c r="H14" t="n">
+        <v>4.64</v>
+      </c>
+      <c r="I14" t="n">
+        <v>13.12</v>
+      </c>
+      <c r="J14" t="n">
+        <v>13.54</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15">
+        <f>COUNT(B2:B14) &amp; " / " &amp; 13</f>
+        <v/>
+      </c>
+      <c r="B15">
+        <f>AVERAGE(B2:B14)</f>
+        <v/>
+      </c>
+      <c r="C15">
+        <f>AVERAGE(C2:C14)</f>
+        <v/>
+      </c>
+      <c r="D15">
+        <f>AVERAGE(D2:D14)</f>
+        <v/>
+      </c>
+      <c r="E15">
+        <f>AVERAGE(E2:E14)</f>
+        <v/>
+      </c>
+      <c r="F15">
+        <f>AVERAGE(F2:F14)</f>
+        <v/>
+      </c>
+      <c r="G15">
+        <f>AVERAGE(G2:G14)</f>
+        <v/>
+      </c>
+      <c r="H15">
+        <f>AVERAGE(H2:H14)</f>
+        <v/>
+      </c>
+      <c r="I15">
+        <f>AVERAGE(I2:I14)</f>
+        <v/>
+      </c>
+      <c r="J15">
+        <f>AVERAGE(J2:J14)</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="65" customWidth="1" min="1" max="1"/>
+    <col width="44" customWidth="1" min="2" max="2"/>
+    <col width="43" customWidth="1" min="3" max="3"/>
+    <col width="27" customWidth="1" min="4" max="4"/>
+    <col width="26" customWidth="1" min="5" max="5"/>
+    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="11" customWidth="1" min="7" max="7"/>
+    <col width="14" customWidth="1" min="8" max="8"/>
+    <col width="13" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Filename</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>PSNR Ground checker diff Reference checker</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>PSNR Ground checker diff Enhanced checker</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Reference</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Enhanced</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Dehazed</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>AG Ground</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>AG Reference</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>AG Enhanced</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>AG Dehazed</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Beside_Camera_light10_exp43294.0_20242111_115040.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Beside_Camera_light5_exp67607.0_20242111_115120.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Green_Beside_Camera_light10_exp80259.0_20242111_115244.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Green_Beside_Camera_light5_exp111285.0_20242111_115220.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Green_InFront_Camera_light10_exp59741.0_20242111_115736.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Green_InFront_Camera_light5_exp89059.0_20242111_115712.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Green_Right_Side_light10_exp73625.0_20242111_115328.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Green_Right_Side_light5_exp98096.0_20242111_115353.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>InFront_Camera_light10_exp25696.0_20242111_115545.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>InFront_Camera_light5_exp45698.0_20242111_115608.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Right_Side_light10_exp31992.0_20242111_115453.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Right_Side_light5_exp52570.0_20242111_115428.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Test_lightAmbient_exp293131.0_20242111_115850.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Underwater_Beside_Camera_lightx_exp125944.0_20242111_115811.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16">
+        <f>COUNT(B2:B15) &amp; " / " &amp; 14</f>
+        <v/>
+      </c>
+      <c r="B16">
+        <f>AVERAGE(B2:B15)</f>
+        <v/>
+      </c>
+      <c r="C16">
+        <f>AVERAGE(C2:C15)</f>
+        <v/>
+      </c>
+      <c r="D16">
+        <f>AVERAGE(D2:D15)</f>
+        <v/>
+      </c>
+      <c r="E16">
+        <f>AVERAGE(E2:E15)</f>
+        <v/>
+      </c>
+      <c r="F16">
+        <f>AVERAGE(F2:F15)</f>
+        <v/>
+      </c>
+      <c r="G16">
+        <f>AVERAGE(G2:G15)</f>
+        <v/>
+      </c>
+      <c r="H16">
+        <f>AVERAGE(H2:H15)</f>
+        <v/>
+      </c>
+      <c r="I16">
+        <f>AVERAGE(I2:I15)</f>
+        <v/>
+      </c>
+      <c r="J16">
+        <f>AVERAGE(J2:J15)</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="64" customWidth="1" min="1" max="1"/>
+    <col width="44" customWidth="1" min="2" max="2"/>
+    <col width="43" customWidth="1" min="3" max="3"/>
+    <col width="27" customWidth="1" min="4" max="4"/>
+    <col width="26" customWidth="1" min="5" max="5"/>
+    <col width="25" customWidth="1" min="6" max="6"/>
+    <col width="11" customWidth="1" min="7" max="7"/>
+    <col width="14" customWidth="1" min="8" max="8"/>
+    <col width="13" customWidth="1" min="9" max="9"/>
+    <col width="12" customWidth="1" min="10" max="10"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Filename</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>PSNR Ground checker diff Reference checker</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>PSNR Ground checker diff Enhanced checker</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Reference</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Enhanced</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>MBE Ground diff Dehazed</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>AG Ground</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>AG Reference</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>AG Enhanced</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>AG Dehazed</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Beside_Camera_light10_exp16519.0_20242111_110824.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Beside_Camera_light5_exp23272.0_20242111_110848.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>InFront_Camera_light10_exp17750.0_20242111_111055.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>InFront_Camera_light5_exp22120.0_20242111_111130.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Right_Side_light10_exp17889.0_20242111_111007.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Right_Side_light5_exp32389.0_20242111_110939.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Underwater_Beside_Camera_lightx_exp93707.0_20242111_111244.png</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9">
+        <f>COUNT(B2:B8) &amp; " / " &amp; 7</f>
+        <v/>
+      </c>
+      <c r="B9">
+        <f>AVERAGE(B2:B8)</f>
+        <v/>
+      </c>
+      <c r="C9">
+        <f>AVERAGE(C2:C8)</f>
+        <v/>
+      </c>
+      <c r="D9">
+        <f>AVERAGE(D2:D8)</f>
+        <v/>
+      </c>
+      <c r="E9">
+        <f>AVERAGE(E2:E8)</f>
+        <v/>
+      </c>
+      <c r="F9">
+        <f>AVERAGE(F2:F8)</f>
+        <v/>
+      </c>
+      <c r="G9">
+        <f>AVERAGE(G2:G8)</f>
+        <v/>
+      </c>
+      <c r="H9">
+        <f>AVERAGE(H2:H8)</f>
+        <v/>
+      </c>
+      <c r="I9">
+        <f>AVERAGE(I2:I8)</f>
+        <v/>
+      </c>
+      <c r="J9">
+        <f>AVERAGE(J2:J8)</f>
+        <v/>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>